<commit_message>
test case template added
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganes\git\Sample\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B6DA8A-04E7-497D-8E26-839A680856A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,43 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>S.No</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>Test Description</t>
+  </si>
+  <si>
+    <t>Test Priority</t>
+  </si>
+  <si>
+    <t>Test Steps</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -37,7 +78,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +86,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +387,284 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>